<commit_message>
completed worksheets making and adding income and expenses
</commit_message>
<xml_diff>
--- a/sheets/income_sheet_day.xlsx
+++ b/sheets/income_sheet_day.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet name="Income Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Income Sheet'!$A$1:$E$2</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -34,10 +37,22 @@
     <t>2024-08-08</t>
   </si>
   <si>
+    <t>bro</t>
+  </si>
+  <si>
     <t>test</t>
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Min</t>
   </si>
 </sst>
 </file>
@@ -46,12 +61,20 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="$#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -65,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -74,13 +97,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD7E4BC"/>
+        <fgColor rgb="FF4F81BD"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCE6F1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -112,17 +141,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
@@ -412,15 +463,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -447,26 +503,59 @@
       <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>6</v>
       </c>
       <c r="D2" s="3">
         <v>500</v>
       </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="4">
         <f>SUM(D2:D2)</f>
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:5">
+      <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5">
+        <f>AVERAGE(D2:D2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5">
+        <f>MAX(D2:D2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5">
+        <f>MIN(D2:D2)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:E2"/>
+  <conditionalFormatting sqref="D2">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>1000</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>